<commit_message>
Finished summarizer + tests
Need to tune parameters to provide better final summary
</commit_message>
<xml_diff>
--- a/data/chunk_search/chunks_2.xlsx
+++ b/data/chunk_search/chunks_2.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/j_yaacoub_mail_utoronto_ca/Documents/Code/CSR_summarizer/data/chunk_search/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_23F921ED61CBCE16CB2C4C038DD5A03754BA61D3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F06F4B49-65C1-411C-9D75-3CD0E916035D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -417,8 +423,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,10 +476,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,6 +490,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -527,7 +544,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -559,9 +576,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,6 +628,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -768,14 +821,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="131.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -789,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>22</v>
       </c>
@@ -803,10 +861,10 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>0.3901331579053889</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>0.39013315790538888</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>39</v>
       </c>
@@ -820,10 +878,10 @@
         <v>12</v>
       </c>
       <c r="E3">
-        <v>0.3899710356893203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>0.38997103568932029</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>25</v>
       </c>
@@ -837,10 +895,10 @@
         <v>8</v>
       </c>
       <c r="E4">
-        <v>0.3838628577425185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>0.38386285774251849</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>38</v>
       </c>
@@ -854,10 +912,10 @@
         <v>11</v>
       </c>
       <c r="E5">
-        <v>0.3826259177090702</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>0.38262591770907017</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -871,10 +929,10 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.3798839785310507</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>0.37988397853105071</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>24</v>
       </c>
@@ -888,10 +946,10 @@
         <v>7</v>
       </c>
       <c r="E7">
-        <v>0.3760663972312016</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>0.37606639723120161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>40</v>
       </c>
@@ -905,10 +963,10 @@
         <v>13</v>
       </c>
       <c r="E8">
-        <v>0.3745198360216008</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>0.37451983602160083</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>41</v>
       </c>
@@ -922,10 +980,10 @@
         <v>14</v>
       </c>
       <c r="E9">
-        <v>0.3715521868867003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>0.37155218688670028</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -939,10 +997,10 @@
         <v>4</v>
       </c>
       <c r="E10">
-        <v>0.3715186243793023</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>0.37151862437930228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>26</v>
       </c>
@@ -956,10 +1014,10 @@
         <v>9</v>
       </c>
       <c r="E11">
-        <v>0.3634994506141327</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>0.36349945061413269</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>18</v>
       </c>
@@ -973,10 +1031,10 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>0.3601873205952534</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>0.36018732059525338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>23</v>
       </c>
@@ -990,10 +1048,10 @@
         <v>6</v>
       </c>
       <c r="E13">
-        <v>0.3583015372690689</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>0.35830153726906888</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -1007,10 +1065,10 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>0.3557332932634107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>0.35573329326341069</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -1024,10 +1082,10 @@
         <v>2</v>
       </c>
       <c r="E15">
-        <v>0.3521694527477168</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>0.35216945274771683</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>33</v>
       </c>
@@ -1041,14 +1099,14 @@
         <v>6</v>
       </c>
       <c r="E16">
-        <v>0.348963031052436</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>0.34896303105243598</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C17" t="s">
@@ -1058,10 +1116,10 @@
         <v>5</v>
       </c>
       <c r="E17">
-        <v>0.3474977875203616</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>0.34749778752036159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>10</v>
       </c>
@@ -1075,14 +1133,14 @@
         <v>3</v>
       </c>
       <c r="E18">
-        <v>0.3461436238817941</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>0.34614362388179409</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>5</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C19" t="s">
@@ -1092,10 +1150,10 @@
         <v>3</v>
       </c>
       <c r="E19">
-        <v>0.3410789000176966</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>0.34107890001769658</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -1109,10 +1167,10 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.3395007969541021</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>0.33950079695410212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -1126,7 +1184,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0.3394933589006008</v>
+        <v>0.33949335890060078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>